<commit_message>
New attributes added for the client and person form, bulk registration uploadn
</commit_message>
<xml_diff>
--- a/src/assets/excel/plantilla_clientes.xlsx
+++ b/src/assets/excel/plantilla_clientes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documentos\Visual Studio 2022\Projects\HSWRISK-FRONT\src\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E24571-6279-4C61-8CDA-AE5BAFC3F7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3516BE34-D544-4FA3-A8FE-2CC0BA50F88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{719DBC3C-A239-47CD-8C00-27B00358B4A4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Clientes" sheetId="1" r:id="rId1"/>
     <sheet name="Listas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
   <si>
     <t>PRIMER-NOMBRE</t>
   </si>
@@ -51,12 +51,12 @@
     <t>SEGUNDO-APELLIDO</t>
   </si>
   <si>
+    <t>TIPO_DOCUMENTO</t>
+  </si>
+  <si>
     <t>DOCUMENTO</t>
   </si>
   <si>
-    <t>TIPO_DOCUMENTO</t>
-  </si>
-  <si>
     <t>DIRECCION</t>
   </si>
   <si>
@@ -66,24 +66,39 @@
     <t>TELEFONO</t>
   </si>
   <si>
+    <t>GENERO</t>
+  </si>
+  <si>
     <t>FECHA-NACIMIENTO</t>
   </si>
   <si>
+    <t>NIVEL DE LECTURA</t>
+  </si>
+  <si>
+    <t>NIVEL DE ESCRITURA</t>
+  </si>
+  <si>
     <t>NIVEL-EDUCATIVO</t>
   </si>
   <si>
     <t>AREA-TRABAJO</t>
   </si>
   <si>
-    <t>CARGO</t>
+    <t>SECTOR ECONOMICO</t>
+  </si>
+  <si>
+    <t>AREA DE TRABAJO</t>
+  </si>
+  <si>
+    <t>CARGO ACTUAL</t>
+  </si>
+  <si>
+    <t>LECTOESCRITURA</t>
   </si>
   <si>
     <t>RH</t>
   </si>
   <si>
-    <t>LECTOESCRITURA</t>
-  </si>
-  <si>
     <t>ALERGIAS</t>
   </si>
   <si>
@@ -99,92 +114,104 @@
     <t>ACUDIENTE</t>
   </si>
   <si>
+    <t>PARENTESCO</t>
+  </si>
+  <si>
     <t>TEL_ACUDIENTE</t>
   </si>
   <si>
-    <t>GENERO</t>
+    <t>PEPITO</t>
+  </si>
+  <si>
+    <t>PEREZ</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>Calle 48 # 24 - 93</t>
+  </si>
+  <si>
+    <t>josepoza125@gmail.com</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>BUENO</t>
+  </si>
+  <si>
+    <t>UNIVERSITARIO</t>
+  </si>
+  <si>
+    <t>SISTEMAS</t>
+  </si>
+  <si>
+    <t>Sector agropecuario</t>
+  </si>
+  <si>
+    <t>ALTURAS</t>
+  </si>
+  <si>
+    <t>AYUDANTE</t>
+  </si>
+  <si>
+    <t>ALFABETA</t>
+  </si>
+  <si>
+    <t>O+</t>
+  </si>
+  <si>
+    <t>NO REFIERE</t>
+  </si>
+  <si>
+    <t>JULANITO PEREZ</t>
+  </si>
+  <si>
+    <t>HERMANO</t>
+  </si>
+  <si>
+    <t>LECTO_ESCRITURA</t>
+  </si>
+  <si>
+    <t>TIPO DOCUMENTO</t>
   </si>
   <si>
     <t>M</t>
   </si>
   <si>
-    <t>CC</t>
-  </si>
-  <si>
-    <t>Calle 48 # 24 - 93</t>
-  </si>
-  <si>
-    <t>josepoza125@gmail.com</t>
-  </si>
-  <si>
-    <t>SISTEMAS</t>
-  </si>
-  <si>
-    <t>AYUDANTE</t>
-  </si>
-  <si>
-    <t>ALFABETA</t>
-  </si>
-  <si>
-    <t>NO REFIERE</t>
-  </si>
-  <si>
-    <t>O+</t>
-  </si>
-  <si>
     <t>PRIMARIA</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>SECUNDARIA</t>
   </si>
   <si>
+    <t>ANALFABETA</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
     <t>TECNICO</t>
   </si>
   <si>
+    <t>PAS</t>
+  </si>
+  <si>
     <t>TECNOLOGO</t>
   </si>
   <si>
-    <t>UNIVERSITARIO</t>
+    <t>CE</t>
   </si>
   <si>
     <t>OTRO</t>
-  </si>
-  <si>
-    <t>TIPO DOCUMENTO</t>
-  </si>
-  <si>
-    <t>TI</t>
-  </si>
-  <si>
-    <t>PAS</t>
-  </si>
-  <si>
-    <t>CE</t>
-  </si>
-  <si>
-    <t>PEPITO</t>
-  </si>
-  <si>
-    <t>PEREZ</t>
-  </si>
-  <si>
-    <t>JULANITO PEREZ</t>
-  </si>
-  <si>
-    <t>LECTO_ESCRITURA</t>
-  </si>
-  <si>
-    <t>ANALFABETA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +238,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -265,7 +300,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -285,9 +320,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -319,6 +351,29 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -339,7 +394,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -635,13 +690,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6192F83-C72F-4B91-8040-CB2C63CF9DBD}">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:AA56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" style="5" bestFit="1" customWidth="1"/>
@@ -649,25 +704,29 @@
     <col min="4" max="4" width="20" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.42578125" style="14"/>
+    <col min="12" max="13" width="19.5703125" style="17" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15" style="17" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" style="5" customWidth="1"/>
+    <col min="18" max="18" width="19.85546875" style="5" customWidth="1"/>
+    <col min="19" max="19" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.28515625" style="17" customWidth="1"/>
+    <col min="27" max="27" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -681,10 +740,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>6</v>
@@ -696,125 +755,336 @@
         <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="W1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
+      <c r="A2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="9">
+        <v>180386971</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="8">
+        <v>3124888633</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="12">
+        <v>44951</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="U2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="V2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="W2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="7" t="s">
+      <c r="Z2" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="10">
-        <v>1003828711</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="9">
-        <v>3124888633</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="13">
-        <v>44951</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="S2" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="U2" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="V2" s="15">
+      <c r="AA2" s="14">
         <v>3134468491</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="K3" s="6"/>
+    <row r="3" spans="1:27">
+      <c r="K3" s="12"/>
+      <c r="M3" s="16"/>
+    </row>
+    <row r="4" spans="1:27">
+      <c r="K4" s="12"/>
+      <c r="M4" s="16"/>
+    </row>
+    <row r="5" spans="1:27">
+      <c r="K5" s="12"/>
+      <c r="M5" s="16"/>
+    </row>
+    <row r="6" spans="1:27">
+      <c r="K6" s="12"/>
+      <c r="M6" s="16"/>
+    </row>
+    <row r="7" spans="1:27">
+      <c r="K7" s="12"/>
+      <c r="M7" s="16"/>
+    </row>
+    <row r="8" spans="1:27">
+      <c r="D8" s="21"/>
+      <c r="K8" s="12"/>
+      <c r="M8" s="16"/>
+    </row>
+    <row r="9" spans="1:27">
+      <c r="K9" s="12"/>
+      <c r="M9" s="16"/>
+    </row>
+    <row r="10" spans="1:27">
+      <c r="K10" s="12"/>
+      <c r="M10" s="16"/>
+    </row>
+    <row r="11" spans="1:27">
+      <c r="K11" s="12"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="16"/>
+    </row>
+    <row r="12" spans="1:27">
+      <c r="K12" s="12"/>
+      <c r="M12" s="16"/>
+    </row>
+    <row r="13" spans="1:27">
+      <c r="K13" s="12"/>
+      <c r="M13" s="16"/>
+    </row>
+    <row r="14" spans="1:27">
+      <c r="K14" s="12"/>
+      <c r="M14" s="16"/>
+    </row>
+    <row r="15" spans="1:27">
+      <c r="K15" s="12"/>
+      <c r="M15" s="16"/>
+    </row>
+    <row r="16" spans="1:27">
+      <c r="K16" s="12"/>
+      <c r="M16" s="16"/>
+    </row>
+    <row r="17" spans="11:13">
+      <c r="K17" s="12"/>
+      <c r="M17" s="16"/>
+    </row>
+    <row r="18" spans="11:13">
+      <c r="M18" s="16"/>
+    </row>
+    <row r="19" spans="11:13">
+      <c r="M19" s="16"/>
+    </row>
+    <row r="20" spans="11:13">
+      <c r="M20" s="16"/>
+    </row>
+    <row r="21" spans="11:13">
+      <c r="M21" s="16"/>
+    </row>
+    <row r="22" spans="11:13">
+      <c r="M22" s="16"/>
+    </row>
+    <row r="23" spans="11:13">
+      <c r="M23" s="16"/>
+    </row>
+    <row r="24" spans="11:13">
+      <c r="M24" s="16"/>
+    </row>
+    <row r="25" spans="11:13">
+      <c r="M25" s="16"/>
+    </row>
+    <row r="26" spans="11:13">
+      <c r="M26" s="16"/>
+    </row>
+    <row r="27" spans="11:13">
+      <c r="M27" s="16"/>
+    </row>
+    <row r="28" spans="11:13">
+      <c r="M28" s="16"/>
+    </row>
+    <row r="29" spans="11:13">
+      <c r="M29" s="16"/>
+    </row>
+    <row r="30" spans="11:13">
+      <c r="M30" s="16"/>
+    </row>
+    <row r="31" spans="11:13">
+      <c r="M31" s="16"/>
+    </row>
+    <row r="32" spans="11:13">
+      <c r="M32" s="16"/>
+    </row>
+    <row r="33" spans="13:13">
+      <c r="M33" s="16"/>
+    </row>
+    <row r="34" spans="13:13">
+      <c r="M34" s="16"/>
+    </row>
+    <row r="35" spans="13:13">
+      <c r="M35" s="16"/>
+    </row>
+    <row r="36" spans="13:13">
+      <c r="M36" s="16"/>
+    </row>
+    <row r="37" spans="13:13">
+      <c r="M37" s="16"/>
+    </row>
+    <row r="38" spans="13:13">
+      <c r="M38" s="16"/>
+    </row>
+    <row r="39" spans="13:13">
+      <c r="M39" s="16"/>
+    </row>
+    <row r="40" spans="13:13">
+      <c r="M40" s="16"/>
+    </row>
+    <row r="41" spans="13:13">
+      <c r="M41" s="16"/>
+    </row>
+    <row r="42" spans="13:13">
+      <c r="M42" s="16"/>
+    </row>
+    <row r="43" spans="13:13">
+      <c r="M43" s="16"/>
+    </row>
+    <row r="44" spans="13:13">
+      <c r="M44" s="16"/>
+    </row>
+    <row r="45" spans="13:13">
+      <c r="M45" s="16"/>
+    </row>
+    <row r="46" spans="13:13">
+      <c r="M46" s="16"/>
+    </row>
+    <row r="47" spans="13:13">
+      <c r="M47" s="16"/>
+    </row>
+    <row r="48" spans="13:13">
+      <c r="M48" s="16"/>
+    </row>
+    <row r="49" spans="13:13">
+      <c r="M49" s="16"/>
+    </row>
+    <row r="50" spans="13:13">
+      <c r="M50" s="16"/>
+    </row>
+    <row r="51" spans="13:13">
+      <c r="M51" s="16"/>
+    </row>
+    <row r="52" spans="13:13">
+      <c r="M52" s="16"/>
+    </row>
+    <row r="53" spans="13:13">
+      <c r="M53" s="16"/>
+    </row>
+    <row r="54" spans="13:13">
+      <c r="M54" s="16"/>
+    </row>
+    <row r="55" spans="13:13">
+      <c r="M55" s="16"/>
+    </row>
+    <row r="56" spans="13:13">
+      <c r="M56" s="16"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="date" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{CA4D1EE6-86C9-448B-9CA1-27E95D40418F}">
-      <formula1>1</formula1>
-      <formula2>402114</formula2>
-    </dataValidation>
+  <dataValidations count="5">
     <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{EBB93CBA-5070-47D8-917E-FEA8F2015C93}">
       <formula1>0</formula1>
       <formula2>1E+42</formula2>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576 V2:V1048576" xr:uid="{4A3A6276-1CBB-46E3-BB32-A0EACE9042DB}">
+    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576 AA2:AA1048576" xr:uid="{4A3A6276-1CBB-46E3-BB32-A0EACE9042DB}">
       <formula1>1</formula1>
       <formula2>1E+43</formula2>
+    </dataValidation>
+    <dataValidation type="date" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576 M2 M4:M1048576" xr:uid="{CA4D1EE6-86C9-448B-9CA1-27E95D40418F}">
+      <formula1>1</formula1>
+      <formula2>402114</formula2>
+    </dataValidation>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L1048576" xr:uid="{1A5B59F0-9785-46EB-9DE1-D369DB28E5E0}"/>
+    <dataValidation type="textLength" errorStyle="warning" operator="notBetween" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3" xr:uid="{70096F4C-BD5E-47B0-9B5A-F51971206066}">
+      <formula1>1</formula1>
+      <formula2>500</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -835,7 +1105,7 @@
           <x14:formula1>
             <xm:f>Listas!$C$2:$C$7</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L1048576</xm:sqref>
+          <xm:sqref>N2:N1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6EF687AF-5499-4F67-BE2A-B0A8D9076AD9}">
           <x14:formula1>
@@ -847,7 +1117,7 @@
           <x14:formula1>
             <xm:f>Listas!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>P2:P1048576</xm:sqref>
+          <xm:sqref>S2:S1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -863,83 +1133,83 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" style="14"/>
-    <col min="3" max="3" width="17.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="14"/>
-    <col min="5" max="5" width="17.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="14"/>
-    <col min="7" max="7" width="17.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="14"/>
+    <col min="1" max="2" width="11.42578125" style="13"/>
+    <col min="3" max="3" width="17.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="13"/>
+    <col min="5" max="5" width="17.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="13"/>
+    <col min="7" max="7" width="17.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="14" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="14" t="s">
+      <c r="C3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="C4" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="C5" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="C6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="14" t="s">
-        <v>37</v>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="C7" s="13" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new input for Company and new requeriments
</commit_message>
<xml_diff>
--- a/src/assets/excel/plantilla_clientes.xlsx
+++ b/src/assets/excel/plantilla_clientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documentos\Visual Studio 2022\Projects\HSWRISK-FRONT\src\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3516BE34-D544-4FA3-A8FE-2CC0BA50F88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4F84B62-36BA-4C2B-AE10-7EF526554938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{719DBC3C-A239-47CD-8C00-27B00358B4A4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
   <si>
     <t>PRIMER-NOMBRE</t>
   </si>
@@ -120,6 +120,9 @@
     <t>TEL_ACUDIENTE</t>
   </si>
   <si>
+    <t>PAÍS DE NACIMIENTO</t>
+  </si>
+  <si>
     <t>PEPITO</t>
   </si>
   <si>
@@ -169,6 +172,9 @@
   </si>
   <si>
     <t>HERMANO</t>
+  </si>
+  <si>
+    <t>COLOMBIA</t>
   </si>
   <si>
     <t>LECTO_ESCRITURA</t>
@@ -690,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6192F83-C72F-4B91-8040-CB2C63CF9DBD}">
-  <dimension ref="A1:AA56"/>
+  <dimension ref="A1:AB56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AB9" sqref="AB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -723,10 +729,11 @@
     <col min="24" max="25" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="16.28515625" style="17" customWidth="1"/>
     <col min="27" max="27" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="11.42578125" style="13"/>
+    <col min="28" max="28" width="16.28515625" style="17" customWidth="1"/>
+    <col min="29" max="16384" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:28">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -808,141 +815,147 @@
       <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:27">
+      <c r="AB1" s="20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28">
       <c r="A2" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F2" s="9">
         <v>180386971</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I2" s="8">
         <v>3124888633</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K2" s="12">
         <v>44951</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q2" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R2" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="T2" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="U2" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V2" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W2" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X2" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y2" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Z2" s="19" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AA2" s="14">
         <v>3134468491</v>
       </c>
-    </row>
-    <row r="3" spans="1:27">
+      <c r="AB2" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28">
       <c r="K3" s="12"/>
       <c r="M3" s="16"/>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:28">
       <c r="K4" s="12"/>
       <c r="M4" s="16"/>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:28">
       <c r="K5" s="12"/>
       <c r="M5" s="16"/>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:28">
       <c r="K6" s="12"/>
       <c r="M6" s="16"/>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:28">
       <c r="K7" s="12"/>
       <c r="M7" s="16"/>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:28">
       <c r="D8" s="21"/>
       <c r="K8" s="12"/>
       <c r="M8" s="16"/>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:28">
       <c r="K9" s="12"/>
       <c r="M9" s="16"/>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:28">
       <c r="K10" s="12"/>
       <c r="M10" s="16"/>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:28">
       <c r="K11" s="12"/>
       <c r="L11" s="18"/>
       <c r="M11" s="16"/>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:28">
       <c r="K12" s="12"/>
       <c r="M12" s="16"/>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:28">
       <c r="K13" s="12"/>
       <c r="M13" s="16"/>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:28">
       <c r="K14" s="12"/>
       <c r="M14" s="16"/>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:28">
       <c r="K15" s="12"/>
       <c r="M15" s="16"/>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:28">
       <c r="K16" s="12"/>
       <c r="M16" s="16"/>
     </row>
@@ -1068,7 +1081,7 @@
       <c r="M56" s="16"/>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{EBB93CBA-5070-47D8-917E-FEA8F2015C93}">
       <formula1>0</formula1>
       <formula2>1E+42</formula2>
@@ -1086,6 +1099,7 @@
       <formula1>1</formula1>
       <formula2>500</formula2>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB1:AB1048576" xr:uid="{C3B0A97B-1A23-40F9-B9F5-7D6DECBF6FF7}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{306C1B34-6D98-4CFF-92A9-4500B27DD4C1}"/>
@@ -1152,64 +1166,64 @@
         <v>13</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="C4" s="13" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="C5" s="13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="C6" s="13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="C7" s="13" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
log out and clean browser
</commit_message>
<xml_diff>
--- a/src/assets/excel/plantilla_clientes.xlsx
+++ b/src/assets/excel/plantilla_clientes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28502"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documentos\Visual Studio 2022\Projects\HSWRISK-FRONT\src\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4F84B62-36BA-4C2B-AE10-7EF526554938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BED96C46-E306-4BE3-8F47-38FD686B7150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{719DBC3C-A239-47CD-8C00-27B00358B4A4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>PRIMER-NOMBRE</t>
   </si>
@@ -69,7 +69,7 @@
     <t>GENERO</t>
   </si>
   <si>
-    <t>FECHA-NACIMIENTO</t>
+    <t>FECHA DE NACIMIENTO</t>
   </si>
   <si>
     <t>NIVEL DE LECTURA</t>
@@ -84,18 +84,9 @@
     <t>AREA-TRABAJO</t>
   </si>
   <si>
-    <t>SECTOR ECONOMICO</t>
-  </si>
-  <si>
-    <t>AREA DE TRABAJO</t>
-  </si>
-  <si>
     <t>CARGO ACTUAL</t>
   </si>
   <si>
-    <t>LECTOESCRITURA</t>
-  </si>
-  <si>
     <t>RH</t>
   </si>
   <si>
@@ -141,6 +132,9 @@
     <t>F</t>
   </si>
   <si>
+    <t>01/05/2004</t>
+  </si>
+  <si>
     <t>BUENO</t>
   </si>
   <si>
@@ -150,43 +144,37 @@
     <t>SISTEMAS</t>
   </si>
   <si>
-    <t>Sector agropecuario</t>
-  </si>
-  <si>
-    <t>ALTURAS</t>
-  </si>
-  <si>
     <t>AYUDANTE</t>
   </si>
   <si>
+    <t>O+</t>
+  </si>
+  <si>
+    <t>NO REFIERE</t>
+  </si>
+  <si>
+    <t>JULANITO PEREZ</t>
+  </si>
+  <si>
+    <t>HERMANO</t>
+  </si>
+  <si>
+    <t>COLOMBIA</t>
+  </si>
+  <si>
+    <t>LECTO_ESCRITURA</t>
+  </si>
+  <si>
+    <t>TIPO DOCUMENTO</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>PRIMARIA</t>
+  </si>
+  <si>
     <t>ALFABETA</t>
-  </si>
-  <si>
-    <t>O+</t>
-  </si>
-  <si>
-    <t>NO REFIERE</t>
-  </si>
-  <si>
-    <t>JULANITO PEREZ</t>
-  </si>
-  <si>
-    <t>HERMANO</t>
-  </si>
-  <si>
-    <t>COLOMBIA</t>
-  </si>
-  <si>
-    <t>LECTO_ESCRITURA</t>
-  </si>
-  <si>
-    <t>TIPO DOCUMENTO</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>PRIMARIA</t>
   </si>
   <si>
     <t>SECUNDARIA</t>
@@ -306,7 +294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -346,9 +334,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -696,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6192F83-C72F-4B91-8040-CB2C63CF9DBD}">
-  <dimension ref="A1:AB56"/>
+  <dimension ref="A1:Y56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AB9" sqref="AB9"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -714,26 +699,23 @@
     <col min="8" max="8" width="25.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="19.5703125" style="17" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="19.5703125" style="16" customWidth="1"/>
     <col min="14" max="14" width="17.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15" style="17" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" style="5" customWidth="1"/>
-    <col min="18" max="18" width="19.85546875" style="5" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.28515625" style="17" customWidth="1"/>
-    <col min="27" max="27" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.28515625" style="17" customWidth="1"/>
-    <col min="29" max="16384" width="11.42578125" style="13"/>
+    <col min="16" max="16" width="19.85546875" style="5" customWidth="1"/>
+    <col min="17" max="17" width="3.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.28515625" style="16" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.28515625" style="16" customWidth="1"/>
+    <col min="26" max="16384" width="11.42578125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -764,13 +746,13 @@
       <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="14" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="4" t="s">
@@ -779,7 +761,7 @@
       <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="3" t="s">
@@ -800,285 +782,267 @@
       <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="20" t="s">
+    </row>
+    <row r="2" spans="1:25">
+      <c r="A2" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28">
-      <c r="A2" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F2" s="9">
-        <v>180386971</v>
+        <v>2222132</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I2" s="8">
         <v>3124888633</v>
       </c>
       <c r="J2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="12">
-        <v>44951</v>
-      </c>
-      <c r="L2" s="16" t="s">
+      <c r="O2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="N2" s="8" t="s">
+      <c r="P2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="Q2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="P2" s="19" t="s">
+      <c r="R2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="10" t="s">
+      <c r="S2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="U2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="10" t="s">
+      <c r="W2" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="X2" s="13">
+        <v>3134468491</v>
+      </c>
+      <c r="Y2" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="U2" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="V2" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="W2" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="X2" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z2" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA2" s="14">
-        <v>3134468491</v>
-      </c>
-      <c r="AB2" s="19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28">
-      <c r="K3" s="12"/>
-      <c r="M3" s="16"/>
-    </row>
-    <row r="4" spans="1:28">
-      <c r="K4" s="12"/>
-      <c r="M4" s="16"/>
-    </row>
-    <row r="5" spans="1:28">
-      <c r="K5" s="12"/>
-      <c r="M5" s="16"/>
-    </row>
-    <row r="6" spans="1:28">
-      <c r="K6" s="12"/>
-      <c r="M6" s="16"/>
-    </row>
-    <row r="7" spans="1:28">
-      <c r="K7" s="12"/>
-      <c r="M7" s="16"/>
-    </row>
-    <row r="8" spans="1:28">
-      <c r="D8" s="21"/>
-      <c r="K8" s="12"/>
-      <c r="M8" s="16"/>
-    </row>
-    <row r="9" spans="1:28">
-      <c r="K9" s="12"/>
-      <c r="M9" s="16"/>
-    </row>
-    <row r="10" spans="1:28">
-      <c r="K10" s="12"/>
-      <c r="M10" s="16"/>
-    </row>
-    <row r="11" spans="1:28">
-      <c r="K11" s="12"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="16"/>
-    </row>
-    <row r="12" spans="1:28">
-      <c r="K12" s="12"/>
-      <c r="M12" s="16"/>
-    </row>
-    <row r="13" spans="1:28">
-      <c r="K13" s="12"/>
-      <c r="M13" s="16"/>
-    </row>
-    <row r="14" spans="1:28">
-      <c r="K14" s="12"/>
-      <c r="M14" s="16"/>
-    </row>
-    <row r="15" spans="1:28">
-      <c r="K15" s="12"/>
-      <c r="M15" s="16"/>
-    </row>
-    <row r="16" spans="1:28">
-      <c r="K16" s="12"/>
-      <c r="M16" s="16"/>
+    </row>
+    <row r="3" spans="1:25">
+      <c r="K3" s="15"/>
+      <c r="M3" s="15"/>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="K4" s="15"/>
+      <c r="M4" s="15"/>
+    </row>
+    <row r="5" spans="1:25">
+      <c r="K5" s="15"/>
+      <c r="M5" s="15"/>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="K6" s="15"/>
+      <c r="M6" s="15"/>
+    </row>
+    <row r="7" spans="1:25">
+      <c r="K7" s="15"/>
+      <c r="M7" s="15"/>
+    </row>
+    <row r="8" spans="1:25">
+      <c r="D8" s="20"/>
+      <c r="K8" s="15"/>
+      <c r="M8" s="15"/>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="K9" s="15"/>
+      <c r="M9" s="15"/>
+    </row>
+    <row r="10" spans="1:25">
+      <c r="K10" s="15"/>
+      <c r="M10" s="15"/>
+    </row>
+    <row r="11" spans="1:25">
+      <c r="K11" s="15"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="15"/>
+    </row>
+    <row r="12" spans="1:25">
+      <c r="K12" s="15"/>
+      <c r="M12" s="15"/>
+    </row>
+    <row r="13" spans="1:25">
+      <c r="K13" s="15"/>
+      <c r="M13" s="15"/>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="K14" s="15"/>
+      <c r="M14" s="15"/>
+    </row>
+    <row r="15" spans="1:25">
+      <c r="K15" s="15"/>
+      <c r="M15" s="15"/>
+    </row>
+    <row r="16" spans="1:25">
+      <c r="K16" s="15"/>
+      <c r="M16" s="15"/>
     </row>
     <row r="17" spans="11:13">
-      <c r="K17" s="12"/>
-      <c r="M17" s="16"/>
+      <c r="K17" s="15"/>
+      <c r="M17" s="15"/>
     </row>
     <row r="18" spans="11:13">
-      <c r="M18" s="16"/>
+      <c r="M18" s="15"/>
     </row>
     <row r="19" spans="11:13">
-      <c r="M19" s="16"/>
+      <c r="M19" s="15"/>
     </row>
     <row r="20" spans="11:13">
-      <c r="M20" s="16"/>
+      <c r="M20" s="15"/>
     </row>
     <row r="21" spans="11:13">
-      <c r="M21" s="16"/>
+      <c r="M21" s="15"/>
     </row>
     <row r="22" spans="11:13">
-      <c r="M22" s="16"/>
+      <c r="M22" s="15"/>
     </row>
     <row r="23" spans="11:13">
-      <c r="M23" s="16"/>
+      <c r="M23" s="15"/>
     </row>
     <row r="24" spans="11:13">
-      <c r="M24" s="16"/>
+      <c r="M24" s="15"/>
     </row>
     <row r="25" spans="11:13">
-      <c r="M25" s="16"/>
+      <c r="M25" s="15"/>
     </row>
     <row r="26" spans="11:13">
-      <c r="M26" s="16"/>
+      <c r="M26" s="15"/>
     </row>
     <row r="27" spans="11:13">
-      <c r="M27" s="16"/>
+      <c r="M27" s="15"/>
     </row>
     <row r="28" spans="11:13">
-      <c r="M28" s="16"/>
+      <c r="M28" s="15"/>
     </row>
     <row r="29" spans="11:13">
-      <c r="M29" s="16"/>
+      <c r="M29" s="15"/>
     </row>
     <row r="30" spans="11:13">
-      <c r="M30" s="16"/>
+      <c r="M30" s="15"/>
     </row>
     <row r="31" spans="11:13">
-      <c r="M31" s="16"/>
+      <c r="M31" s="15"/>
     </row>
     <row r="32" spans="11:13">
-      <c r="M32" s="16"/>
+      <c r="M32" s="15"/>
     </row>
     <row r="33" spans="13:13">
-      <c r="M33" s="16"/>
+      <c r="M33" s="15"/>
     </row>
     <row r="34" spans="13:13">
-      <c r="M34" s="16"/>
+      <c r="M34" s="15"/>
     </row>
     <row r="35" spans="13:13">
-      <c r="M35" s="16"/>
+      <c r="M35" s="15"/>
     </row>
     <row r="36" spans="13:13">
-      <c r="M36" s="16"/>
+      <c r="M36" s="15"/>
     </row>
     <row r="37" spans="13:13">
-      <c r="M37" s="16"/>
+      <c r="M37" s="15"/>
     </row>
     <row r="38" spans="13:13">
-      <c r="M38" s="16"/>
+      <c r="M38" s="15"/>
     </row>
     <row r="39" spans="13:13">
-      <c r="M39" s="16"/>
+      <c r="M39" s="15"/>
     </row>
     <row r="40" spans="13:13">
-      <c r="M40" s="16"/>
+      <c r="M40" s="15"/>
     </row>
     <row r="41" spans="13:13">
-      <c r="M41" s="16"/>
+      <c r="M41" s="15"/>
     </row>
     <row r="42" spans="13:13">
-      <c r="M42" s="16"/>
+      <c r="M42" s="15"/>
     </row>
     <row r="43" spans="13:13">
-      <c r="M43" s="16"/>
+      <c r="M43" s="15"/>
     </row>
     <row r="44" spans="13:13">
-      <c r="M44" s="16"/>
+      <c r="M44" s="15"/>
     </row>
     <row r="45" spans="13:13">
-      <c r="M45" s="16"/>
+      <c r="M45" s="15"/>
     </row>
     <row r="46" spans="13:13">
-      <c r="M46" s="16"/>
+      <c r="M46" s="15"/>
     </row>
     <row r="47" spans="13:13">
-      <c r="M47" s="16"/>
+      <c r="M47" s="15"/>
     </row>
     <row r="48" spans="13:13">
-      <c r="M48" s="16"/>
+      <c r="M48" s="15"/>
     </row>
     <row r="49" spans="13:13">
-      <c r="M49" s="16"/>
+      <c r="M49" s="15"/>
     </row>
     <row r="50" spans="13:13">
-      <c r="M50" s="16"/>
+      <c r="M50" s="15"/>
     </row>
     <row r="51" spans="13:13">
-      <c r="M51" s="16"/>
+      <c r="M51" s="15"/>
     </row>
     <row r="52" spans="13:13">
-      <c r="M52" s="16"/>
+      <c r="M52" s="15"/>
     </row>
     <row r="53" spans="13:13">
-      <c r="M53" s="16"/>
+      <c r="M53" s="15"/>
     </row>
     <row r="54" spans="13:13">
-      <c r="M54" s="16"/>
+      <c r="M54" s="15"/>
     </row>
     <row r="55" spans="13:13">
-      <c r="M55" s="16"/>
+      <c r="M55" s="15"/>
     </row>
     <row r="56" spans="13:13">
-      <c r="M56" s="16"/>
+      <c r="M56" s="15"/>
     </row>
   </sheetData>
   <dataValidations count="6">
@@ -1086,11 +1050,11 @@
       <formula1>0</formula1>
       <formula2>1E+42</formula2>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576 AA2:AA1048576" xr:uid="{4A3A6276-1CBB-46E3-BB32-A0EACE9042DB}">
+    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576 X2:X1048576" xr:uid="{4A3A6276-1CBB-46E3-BB32-A0EACE9042DB}">
       <formula1>1</formula1>
       <formula2>1E+43</formula2>
     </dataValidation>
-    <dataValidation type="date" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576 M2 M4:M1048576" xr:uid="{CA4D1EE6-86C9-448B-9CA1-27E95D40418F}">
+    <dataValidation type="date" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M4:M1048576 M2" xr:uid="{CA4D1EE6-86C9-448B-9CA1-27E95D40418F}">
       <formula1>1</formula1>
       <formula2>402114</formula2>
     </dataValidation>
@@ -1099,7 +1063,7 @@
       <formula1>1</formula1>
       <formula2>500</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB1:AB1048576" xr:uid="{C3B0A97B-1A23-40F9-B9F5-7D6DECBF6FF7}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y1:Y1048576 K1:K1048576" xr:uid="{C3B0A97B-1A23-40F9-B9F5-7D6DECBF6FF7}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{306C1B34-6D98-4CFF-92A9-4500B27DD4C1}"/>
@@ -1108,7 +1072,7 @@
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5D8080A7-E462-4F23-86C9-F3C047B5C29D}">
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
@@ -1127,12 +1091,6 @@
           </x14:formula1>
           <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CF241144-B31F-43C9-B128-EB817E870FC2}">
-          <x14:formula1>
-            <xm:f>Listas!$E$2:$E$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>S2:S1048576</xm:sqref>
-        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1149,81 +1107,81 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" style="13"/>
-    <col min="3" max="3" width="17.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="13"/>
-    <col min="5" max="5" width="17.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="13"/>
-    <col min="7" max="7" width="17.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="13"/>
+    <col min="1" max="2" width="11.42578125" style="12"/>
+    <col min="3" max="3" width="17.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="12"/>
+    <col min="5" max="5" width="17.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="12"/>
+    <col min="7" max="7" width="17.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="13" t="s">
+      <c r="G3" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="13" t="s">
+    </row>
+    <row r="4" spans="1:7">
+      <c r="C4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="13" t="s">
+      <c r="G4" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="C5" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="C6" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="C4" s="13" t="s">
+    </row>
+    <row r="7" spans="1:7">
+      <c r="C7" s="12" t="s">
         <v>53</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="C5" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="C6" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="C7" s="13" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished logic and management the orders and alert
</commit_message>
<xml_diff>
--- a/src/assets/excel/plantilla_clientes.xlsx
+++ b/src/assets/excel/plantilla_clientes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documentos\Visual Studio 2022\Projects\HSWRISK-FRONT\src\assets\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\EmpresaSigec\HSWRISK-FRONT\src\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BED96C46-E306-4BE3-8F47-38FD686B7150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D1EF48-DE74-4BDC-B691-9D9057068243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{719DBC3C-A239-47CD-8C00-27B00358B4A4}"/>
+    <workbookView xWindow="-20520" yWindow="1440" windowWidth="20640" windowHeight="11040" xr2:uid="{719DBC3C-A239-47CD-8C00-27B00358B4A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Clientes" sheetId="1" r:id="rId1"/>
@@ -189,9 +189,6 @@
     <t>TECNICO</t>
   </si>
   <si>
-    <t>PAS</t>
-  </si>
-  <si>
     <t>TECNOLOGO</t>
   </si>
   <si>
@@ -199,13 +196,16 @@
   </si>
   <si>
     <t>OTRO</t>
+  </si>
+  <si>
+    <t>PPT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,7 +294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -364,6 +364,12 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -385,9 +391,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -425,7 +431,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -531,7 +537,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -673,7 +679,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -683,39 +689,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6192F83-C72F-4B91-8040-CB2C63CF9DBD}">
   <dimension ref="A1:Y56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P1048576"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.54296875" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="19.5703125" style="16" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.54296875" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="19.54296875" style="16" customWidth="1"/>
+    <col min="14" max="14" width="17.81640625" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.85546875" style="5" customWidth="1"/>
-    <col min="17" max="17" width="3.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.28515625" style="16" customWidth="1"/>
-    <col min="24" max="24" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.28515625" style="16" customWidth="1"/>
-    <col min="26" max="16384" width="11.42578125" style="12"/>
+    <col min="16" max="16" width="19.81640625" style="5" customWidth="1"/>
+    <col min="17" max="17" width="3.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="16.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.26953125" style="16" customWidth="1"/>
+    <col min="24" max="24" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.26953125" style="16" customWidth="1"/>
+    <col min="26" max="16384" width="11.453125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -792,7 +798,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>25</v>
       </c>
@@ -802,7 +808,7 @@
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="8" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="F2" s="9">
         <v>2222132</v>
@@ -865,183 +871,184 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="K3" s="15"/>
       <c r="M3" s="15"/>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="K4" s="15"/>
       <c r="M4" s="15"/>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="E5" s="20"/>
       <c r="K5" s="15"/>
       <c r="M5" s="15"/>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="K6" s="15"/>
       <c r="M6" s="15"/>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="K7" s="15"/>
       <c r="M7" s="15"/>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="D8" s="20"/>
       <c r="K8" s="15"/>
       <c r="M8" s="15"/>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="K9" s="15"/>
       <c r="M9" s="15"/>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="K10" s="15"/>
       <c r="M10" s="15"/>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="K11" s="15"/>
       <c r="L11" s="17"/>
       <c r="M11" s="15"/>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="K12" s="15"/>
       <c r="M12" s="15"/>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="K13" s="15"/>
       <c r="M13" s="15"/>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="K14" s="15"/>
       <c r="M14" s="15"/>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="K15" s="15"/>
       <c r="M15" s="15"/>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="K16" s="15"/>
       <c r="M16" s="15"/>
     </row>
-    <row r="17" spans="11:13">
+    <row r="17" spans="11:13" x14ac:dyDescent="0.35">
       <c r="K17" s="15"/>
       <c r="M17" s="15"/>
     </row>
-    <row r="18" spans="11:13">
+    <row r="18" spans="11:13" x14ac:dyDescent="0.35">
       <c r="M18" s="15"/>
     </row>
-    <row r="19" spans="11:13">
+    <row r="19" spans="11:13" x14ac:dyDescent="0.35">
       <c r="M19" s="15"/>
     </row>
-    <row r="20" spans="11:13">
+    <row r="20" spans="11:13" x14ac:dyDescent="0.35">
       <c r="M20" s="15"/>
     </row>
-    <row r="21" spans="11:13">
+    <row r="21" spans="11:13" x14ac:dyDescent="0.35">
       <c r="M21" s="15"/>
     </row>
-    <row r="22" spans="11:13">
+    <row r="22" spans="11:13" x14ac:dyDescent="0.35">
       <c r="M22" s="15"/>
     </row>
-    <row r="23" spans="11:13">
+    <row r="23" spans="11:13" x14ac:dyDescent="0.35">
       <c r="M23" s="15"/>
     </row>
-    <row r="24" spans="11:13">
+    <row r="24" spans="11:13" x14ac:dyDescent="0.35">
       <c r="M24" s="15"/>
     </row>
-    <row r="25" spans="11:13">
+    <row r="25" spans="11:13" x14ac:dyDescent="0.35">
       <c r="M25" s="15"/>
     </row>
-    <row r="26" spans="11:13">
+    <row r="26" spans="11:13" x14ac:dyDescent="0.35">
       <c r="M26" s="15"/>
     </row>
-    <row r="27" spans="11:13">
+    <row r="27" spans="11:13" x14ac:dyDescent="0.35">
       <c r="M27" s="15"/>
     </row>
-    <row r="28" spans="11:13">
+    <row r="28" spans="11:13" x14ac:dyDescent="0.35">
       <c r="M28" s="15"/>
     </row>
-    <row r="29" spans="11:13">
+    <row r="29" spans="11:13" x14ac:dyDescent="0.35">
       <c r="M29" s="15"/>
     </row>
-    <row r="30" spans="11:13">
+    <row r="30" spans="11:13" x14ac:dyDescent="0.35">
       <c r="M30" s="15"/>
     </row>
-    <row r="31" spans="11:13">
+    <row r="31" spans="11:13" x14ac:dyDescent="0.35">
       <c r="M31" s="15"/>
     </row>
-    <row r="32" spans="11:13">
+    <row r="32" spans="11:13" x14ac:dyDescent="0.35">
       <c r="M32" s="15"/>
     </row>
-    <row r="33" spans="13:13">
+    <row r="33" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M33" s="15"/>
     </row>
-    <row r="34" spans="13:13">
+    <row r="34" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M34" s="15"/>
     </row>
-    <row r="35" spans="13:13">
+    <row r="35" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M35" s="15"/>
     </row>
-    <row r="36" spans="13:13">
+    <row r="36" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M36" s="15"/>
     </row>
-    <row r="37" spans="13:13">
+    <row r="37" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M37" s="15"/>
     </row>
-    <row r="38" spans="13:13">
+    <row r="38" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M38" s="15"/>
     </row>
-    <row r="39" spans="13:13">
+    <row r="39" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M39" s="15"/>
     </row>
-    <row r="40" spans="13:13">
+    <row r="40" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M40" s="15"/>
     </row>
-    <row r="41" spans="13:13">
+    <row r="41" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M41" s="15"/>
     </row>
-    <row r="42" spans="13:13">
+    <row r="42" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M42" s="15"/>
     </row>
-    <row r="43" spans="13:13">
+    <row r="43" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M43" s="15"/>
     </row>
-    <row r="44" spans="13:13">
+    <row r="44" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M44" s="15"/>
     </row>
-    <row r="45" spans="13:13">
+    <row r="45" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M45" s="15"/>
     </row>
-    <row r="46" spans="13:13">
+    <row r="46" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M46" s="15"/>
     </row>
-    <row r="47" spans="13:13">
+    <row r="47" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M47" s="15"/>
     </row>
-    <row r="48" spans="13:13">
+    <row r="48" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M48" s="15"/>
     </row>
-    <row r="49" spans="13:13">
+    <row r="49" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M49" s="15"/>
     </row>
-    <row r="50" spans="13:13">
+    <row r="50" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M50" s="15"/>
     </row>
-    <row r="51" spans="13:13">
+    <row r="51" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M51" s="15"/>
     </row>
-    <row r="52" spans="13:13">
+    <row r="52" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M52" s="15"/>
     </row>
-    <row r="53" spans="13:13">
+    <row r="53" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M53" s="15"/>
     </row>
-    <row r="54" spans="13:13">
+    <row r="54" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M54" s="15"/>
     </row>
-    <row r="55" spans="13:13">
+    <row r="55" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M55" s="15"/>
     </row>
-    <row r="56" spans="13:13">
+    <row r="56" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M56" s="15"/>
     </row>
   </sheetData>
@@ -1099,24 +1106,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE239ACA-D77C-4A7E-AB6C-03221AB43D37}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" style="12"/>
-    <col min="3" max="3" width="17.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="12"/>
-    <col min="5" max="5" width="17.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="12"/>
-    <col min="7" max="7" width="17.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="12"/>
+    <col min="1" max="2" width="11.453125" style="12"/>
+    <col min="3" max="3" width="17.26953125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" style="12"/>
+    <col min="5" max="5" width="17.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" style="12"/>
+    <col min="7" max="7" width="17.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.453125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
@@ -1130,7 +1137,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>43</v>
       </c>
@@ -1144,7 +1151,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>30</v>
       </c>
@@ -1158,31 +1165,35 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C4" s="12" t="s">
         <v>49</v>
       </c>
       <c r="G4" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C5" s="12" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="C5" s="12" t="s">
+      <c r="G5" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C6" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="21"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C7" s="12" t="s">
-        <v>53</v>
-      </c>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D14" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>